<commit_message>
Changed T7.1 Croplands to T7.1 Annual croplands.
</commit_message>
<xml_diff>
--- a/crosswalks/ALUM-IUCNGET/ALUM-IUCNGET.xlsx
+++ b/crosswalks/ALUM-IUCNGET/ALUM-IUCNGET.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE740C0-8789-45AB-9FA7-03AB9D99D211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ECE107-4416-4B4A-8A02-564A88018B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5623" uniqueCount="1491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5623" uniqueCount="1492">
   <si>
     <t>Perennial horticulture</t>
   </si>
@@ -4734,6 +4734,9 @@
   </si>
   <si>
     <t>alum:Intensive-uses</t>
+  </si>
+  <si>
+    <t>T7.1 Annual croplands</t>
   </si>
 </sst>
 </file>
@@ -5737,6 +5740,9 @@
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5766,9 +5772,6 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -6210,25 +6213,25 @@
     </row>
     <row r="2" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="165" t="s">
         <v>993</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="164"/>
-      <c r="I2" s="164"/>
-      <c r="J2" s="164"/>
-      <c r="K2" s="164"/>
-      <c r="L2" s="164"/>
-      <c r="M2" s="164"/>
-      <c r="N2" s="164"/>
-      <c r="O2" s="164"/>
-      <c r="P2" s="164"/>
-      <c r="Q2" s="164"/>
-      <c r="R2" s="164"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
+      <c r="J2" s="165"/>
+      <c r="K2" s="165"/>
+      <c r="L2" s="165"/>
+      <c r="M2" s="165"/>
+      <c r="N2" s="165"/>
+      <c r="O2" s="165"/>
+      <c r="P2" s="165"/>
+      <c r="Q2" s="165"/>
+      <c r="R2" s="165"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -11458,25 +11461,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>1005</v>
       </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
-      <c r="I1" s="165"/>
-      <c r="J1" s="165"/>
-      <c r="K1" s="165"/>
-      <c r="O1" s="166" t="s">
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="166"/>
+      <c r="O1" s="167" t="s">
         <v>1005</v>
       </c>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="166"/>
-      <c r="R1" s="166"/>
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="167"/>
       <c r="Y1" s="55"/>
       <c r="Z1" s="55"/>
       <c r="AA1" s="55"/>
@@ -11495,10 +11498,10 @@
       <c r="P2" s="126" t="s">
         <v>1007</v>
       </c>
-      <c r="Q2" s="166" t="s">
+      <c r="Q2" s="167" t="s">
         <v>951</v>
       </c>
-      <c r="R2" s="166"/>
+      <c r="R2" s="167"/>
       <c r="Y2" s="131" t="s">
         <v>960</v>
       </c>
@@ -11519,10 +11522,10 @@
       <c r="AO2" s="143" t="s">
         <v>960</v>
       </c>
-      <c r="AP2" s="168" t="s">
+      <c r="AP2" s="169" t="s">
         <v>1007</v>
       </c>
-      <c r="AQ2" s="168"/>
+      <c r="AQ2" s="169"/>
       <c r="AR2" s="144"/>
       <c r="AS2" s="144"/>
       <c r="AT2" s="145" t="s">
@@ -11589,10 +11592,10 @@
       <c r="AS3" s="141" t="s">
         <v>1009</v>
       </c>
-      <c r="AT3" s="167" t="s">
+      <c r="AT3" s="168" t="s">
         <v>946</v>
       </c>
-      <c r="AU3" s="167"/>
+      <c r="AU3" s="168"/>
       <c r="AV3" s="141" t="s">
         <v>947</v>
       </c>
@@ -14782,13 +14785,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="169"/>
-      <c r="B1" s="170"/>
-      <c r="C1" s="171" t="s">
+      <c r="A1" s="170"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="172" t="s">
         <v>659</v>
       </c>
-      <c r="D1" s="172"/>
-      <c r="E1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="174"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
@@ -19846,13 +19849,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="169"/>
-      <c r="B1" s="170"/>
-      <c r="C1" s="171" t="s">
+      <c r="A1" s="170"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="172" t="s">
         <v>659</v>
       </c>
-      <c r="D1" s="172"/>
-      <c r="E1" s="173"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="174"/>
     </row>
     <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="109" t="s">
@@ -23828,8 +23831,8 @@
   <dimension ref="A1:N189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A62" sqref="A62:XFD62"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25176,7 +25179,7 @@
         <v>1482</v>
       </c>
       <c r="E35" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F35" s="154" t="s">
         <v>1033</v>
@@ -25212,7 +25215,7 @@
         <v>1482</v>
       </c>
       <c r="E36" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F36" s="154" t="s">
         <v>1033</v>
@@ -25249,7 +25252,7 @@
         <v>1482</v>
       </c>
       <c r="E37" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F37" s="154" t="s">
         <v>1033</v>
@@ -25286,7 +25289,7 @@
         <v>1482</v>
       </c>
       <c r="E38" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F38" s="154" t="s">
         <v>1033</v>
@@ -25323,7 +25326,7 @@
         <v>1482</v>
       </c>
       <c r="E39" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F39" s="154" t="s">
         <v>1033</v>
@@ -25360,7 +25363,7 @@
         <v>1482</v>
       </c>
       <c r="E40" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F40" s="154" t="s">
         <v>1033</v>
@@ -25397,7 +25400,7 @@
         <v>1482</v>
       </c>
       <c r="E41" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F41" s="154" t="s">
         <v>1033</v>
@@ -25434,7 +25437,7 @@
         <v>1482</v>
       </c>
       <c r="E42" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F42" s="154" t="s">
         <v>1033</v>
@@ -25471,7 +25474,7 @@
         <v>1482</v>
       </c>
       <c r="E43" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F43" s="154" t="s">
         <v>1033</v>
@@ -25508,7 +25511,7 @@
         <v>1482</v>
       </c>
       <c r="E44" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F44" s="154" t="s">
         <v>1033</v>
@@ -25544,7 +25547,7 @@
         <v>1482</v>
       </c>
       <c r="E45" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F45" s="154" t="s">
         <v>1033</v>
@@ -25581,7 +25584,7 @@
         <v>1482</v>
       </c>
       <c r="E46" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F46" s="154" t="s">
         <v>1033</v>
@@ -25618,7 +25621,7 @@
         <v>1482</v>
       </c>
       <c r="E47" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F47" s="154" t="s">
         <v>1033</v>
@@ -25655,7 +25658,7 @@
         <v>1482</v>
       </c>
       <c r="E48" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F48" s="154" t="s">
         <v>1033</v>
@@ -25692,7 +25695,7 @@
         <v>1482</v>
       </c>
       <c r="E49" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F49" s="154" t="s">
         <v>1033</v>
@@ -25729,7 +25732,7 @@
         <v>1482</v>
       </c>
       <c r="E50" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F50" s="154" t="s">
         <v>1033</v>
@@ -25766,7 +25769,7 @@
         <v>1482</v>
       </c>
       <c r="E51" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F51" s="154" t="s">
         <v>1033</v>
@@ -25803,7 +25806,7 @@
         <v>1482</v>
       </c>
       <c r="E52" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F52" s="154" t="s">
         <v>1033</v>
@@ -25840,7 +25843,7 @@
         <v>1482</v>
       </c>
       <c r="E53" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F53" s="154" t="s">
         <v>1033</v>
@@ -25877,7 +25880,7 @@
         <v>1482</v>
       </c>
       <c r="E54" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F54" s="154" t="s">
         <v>1033</v>
@@ -25914,7 +25917,7 @@
         <v>1482</v>
       </c>
       <c r="E55" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F55" s="154" t="s">
         <v>1033</v>
@@ -25951,7 +25954,7 @@
         <v>1482</v>
       </c>
       <c r="E56" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F56" s="154" t="s">
         <v>1033</v>
@@ -26556,7 +26559,7 @@
         <v>1482</v>
       </c>
       <c r="E72" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F72" s="154" t="s">
         <v>1033</v>
@@ -26592,7 +26595,7 @@
         <v>1482</v>
       </c>
       <c r="E73" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F73" s="154" t="s">
         <v>1033</v>
@@ -26629,7 +26632,7 @@
         <v>1482</v>
       </c>
       <c r="E74" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F74" s="154" t="s">
         <v>1033</v>
@@ -26666,7 +26669,7 @@
         <v>1482</v>
       </c>
       <c r="E75" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F75" s="154" t="s">
         <v>1033</v>
@@ -26703,7 +26706,7 @@
         <v>1482</v>
       </c>
       <c r="E76" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F76" s="154" t="s">
         <v>1033</v>
@@ -26740,7 +26743,7 @@
         <v>1482</v>
       </c>
       <c r="E77" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F77" s="154" t="s">
         <v>1033</v>
@@ -26777,7 +26780,7 @@
         <v>1482</v>
       </c>
       <c r="E78" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F78" s="154" t="s">
         <v>1033</v>
@@ -26814,7 +26817,7 @@
         <v>1482</v>
       </c>
       <c r="E79" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F79" s="154" t="s">
         <v>1033</v>
@@ -26851,7 +26854,7 @@
         <v>1482</v>
       </c>
       <c r="E80" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F80" s="154" t="s">
         <v>1033</v>
@@ -26925,7 +26928,7 @@
         <v>1482</v>
       </c>
       <c r="E82" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F82" s="154" t="s">
         <v>1033</v>
@@ -26961,7 +26964,7 @@
         <v>1482</v>
       </c>
       <c r="E83" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F83" s="154" t="s">
         <v>1033</v>
@@ -26998,7 +27001,7 @@
         <v>1482</v>
       </c>
       <c r="E84" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F84" s="154" t="s">
         <v>1033</v>
@@ -27035,7 +27038,7 @@
         <v>1482</v>
       </c>
       <c r="E85" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F85" s="154" t="s">
         <v>1033</v>
@@ -27072,7 +27075,7 @@
         <v>1482</v>
       </c>
       <c r="E86" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F86" s="154" t="s">
         <v>1033</v>
@@ -27109,7 +27112,7 @@
         <v>1482</v>
       </c>
       <c r="E87" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F87" s="154" t="s">
         <v>1033</v>
@@ -27146,7 +27149,7 @@
         <v>1482</v>
       </c>
       <c r="E88" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F88" s="154" t="s">
         <v>1033</v>
@@ -27183,7 +27186,7 @@
         <v>1482</v>
       </c>
       <c r="E89" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F89" s="154" t="s">
         <v>1033</v>
@@ -27220,7 +27223,7 @@
         <v>1482</v>
       </c>
       <c r="E90" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F90" s="154" t="s">
         <v>1033</v>
@@ -27257,7 +27260,7 @@
         <v>1482</v>
       </c>
       <c r="E91" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F91" s="154" t="s">
         <v>1033</v>
@@ -27294,7 +27297,7 @@
         <v>1482</v>
       </c>
       <c r="E92" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F92" s="154" t="s">
         <v>1033</v>
@@ -27331,7 +27334,7 @@
         <v>1482</v>
       </c>
       <c r="E93" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F93" s="154" t="s">
         <v>1033</v>
@@ -27368,7 +27371,7 @@
         <v>1482</v>
       </c>
       <c r="E94" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F94" s="154" t="s">
         <v>1033</v>
@@ -27405,7 +27408,7 @@
         <v>1482</v>
       </c>
       <c r="E95" t="s">
-        <v>1011</v>
+        <v>1491</v>
       </c>
       <c r="F95" s="154" t="s">
         <v>1033</v>
@@ -27635,7 +27638,7 @@
       <c r="B101" s="17" t="s">
         <v>1489</v>
       </c>
-      <c r="C101" s="174" t="s">
+      <c r="C101" s="164" t="s">
         <v>1030</v>
       </c>
       <c r="D101" s="17" t="s">
@@ -30986,6 +30989,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC29B5BE6945C34F8C7CB81794666E31" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f7151ef105987b2d3758ef53560e213">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48c5b5cd9b8d25ff6dd15848836f4270" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -31117,25 +31138,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97EDE51C-194A-4D85-AD03-32004056A6AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -31151,22 +31172,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Better labels on Mapping entities
</commit_message>
<xml_diff>
--- a/crosswalks/ALUM-IUCNGET/ALUM-IUCNGET.xlsx
+++ b/crosswalks/ALUM-IUCNGET/ALUM-IUCNGET.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E524E68-7CD3-4184-A652-69A55EDD8DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CE728B-2C81-44C7-A9F4-650A7F52181D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="5790" windowWidth="23925" windowHeight="10815" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1290" yWindow="9660" windowWidth="34230" windowHeight="10815" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALUM V8" sheetId="5" r:id="rId1"/>
@@ -23211,7 +23211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02CB4D65-9DAF-4373-8A3E-AE42C6AE42AD}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -23271,9 +23271,9 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:N189"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A189"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -23374,13 +23374,13 @@
       </c>
       <c r="M2" s="155"/>
       <c r="N2" s="155" t="str">
-        <f t="shared" ref="N2:N65" si="0">CONCATENATE(B2, " - mapping to IUCN GET")</f>
-        <v>1.1.1 Strict nature reserves - mapping to IUCN GET</v>
+        <f>CONCATENATE(B2, " - mapping to IUCN GET - ", ROW(B2)-1)</f>
+        <v>1.1.1 Strict nature reserves - mapping to IUCN GET - 1</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A66" si="1">_xlfn.CONCAT("alum:",LEFT(B3,FIND(" ",B3)-1))</f>
+        <f t="shared" ref="A3:A66" si="0">_xlfn.CONCAT("alum:",LEFT(B3,FIND(" ",B3)-1))</f>
         <v>alum:1.1.2</v>
       </c>
       <c r="B3" t="s">
@@ -23415,13 +23415,13 @@
       </c>
       <c r="M3" s="155"/>
       <c r="N3" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.1.2 Wilderness area - mapping to IUCN GET</v>
+        <f t="shared" ref="N3:N66" si="1">CONCATENATE(B3, " - mapping to IUCN GET - ", ROW(B3)-1)</f>
+        <v>1.1.2 Wilderness area - mapping to IUCN GET - 2</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.1.3</v>
       </c>
       <c r="B4" t="s">
@@ -23456,13 +23456,13 @@
       </c>
       <c r="M4" s="155"/>
       <c r="N4" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.1.3 National park - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.1.3 National park - mapping to IUCN GET - 3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.1.4</v>
       </c>
       <c r="B5" t="s">
@@ -23497,13 +23497,13 @@
       </c>
       <c r="M5" s="155"/>
       <c r="N5" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.1.4 Natural feature protection - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.1.4 Natural feature protection - mapping to IUCN GET - 4</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.1.5</v>
       </c>
       <c r="B6" t="s">
@@ -23538,13 +23538,13 @@
       </c>
       <c r="M6" s="155"/>
       <c r="N6" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.1.5 Habitat/species management area - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.1.5 Habitat/species management area - mapping to IUCN GET - 5</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.1.6</v>
       </c>
       <c r="B7" t="s">
@@ -23579,13 +23579,13 @@
       </c>
       <c r="M7" s="155"/>
       <c r="N7" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.1.6 Protected landscape - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.1.6 Protected landscape - mapping to IUCN GET - 6</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.1.7</v>
       </c>
       <c r="B8" t="s">
@@ -23620,13 +23620,13 @@
       </c>
       <c r="M8" s="155"/>
       <c r="N8" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.1.7 Other conserved area - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.1.7 Other conserved area - mapping to IUCN GET - 7</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.2.0</v>
       </c>
       <c r="B9" t="s">
@@ -23657,13 +23657,13 @@
         <v>1042</v>
       </c>
       <c r="N9" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.2.0 Managed resource protection - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.2.0 Managed resource protection - mapping to IUCN GET - 8</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.2.1</v>
       </c>
       <c r="B10" t="s">
@@ -23698,13 +23698,13 @@
       </c>
       <c r="M10" s="155"/>
       <c r="N10" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.2.1 Biodiversity - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.2.1 Biodiversity - mapping to IUCN GET - 9</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.2.2</v>
       </c>
       <c r="B11" t="s">
@@ -23739,13 +23739,13 @@
       </c>
       <c r="M11" s="155"/>
       <c r="N11" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.2.2 Surface water supply - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.2.2 Surface water supply - mapping to IUCN GET - 10</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.2.3</v>
       </c>
       <c r="B12" t="s">
@@ -23780,13 +23780,13 @@
       </c>
       <c r="M12" s="155"/>
       <c r="N12" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.2.3 Groundwater - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.2.3 Groundwater - mapping to IUCN GET - 11</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.2.4</v>
       </c>
       <c r="B13" t="s">
@@ -23821,13 +23821,13 @@
       </c>
       <c r="M13" s="155"/>
       <c r="N13" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.2.4 Landscape - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.2.4 Landscape - mapping to IUCN GET - 12</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.2.5</v>
       </c>
       <c r="B14" t="s">
@@ -23862,13 +23862,13 @@
       </c>
       <c r="M14" s="155"/>
       <c r="N14" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.2.5 Traditional indigenous uses - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.2.5 Traditional indigenous uses - mapping to IUCN GET - 13</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.3.0</v>
       </c>
       <c r="B15" t="s">
@@ -23899,13 +23899,13 @@
         <v>1042</v>
       </c>
       <c r="N15" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.3.0 Other minimal use - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.3.0 Other minimal use - mapping to IUCN GET - 14</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.3.1</v>
       </c>
       <c r="B16" t="s">
@@ -23940,13 +23940,13 @@
       </c>
       <c r="M16" s="155"/>
       <c r="N16" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.3.1 Defence land - natural areas - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.3.1 Defence land - natural areas - mapping to IUCN GET - 15</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.3.2</v>
       </c>
       <c r="B17" t="s">
@@ -23981,13 +23981,13 @@
       </c>
       <c r="M17" s="155"/>
       <c r="N17" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.3.2 Stock route - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.3.2 Stock route - mapping to IUCN GET - 16</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.3.3</v>
       </c>
       <c r="B18" t="s">
@@ -24022,13 +24022,13 @@
       </c>
       <c r="M18" s="155"/>
       <c r="N18" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.3.3 Residual native cover - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.3.3 Residual native cover - mapping to IUCN GET - 17</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:1.3.4</v>
       </c>
       <c r="B19" t="s">
@@ -24063,13 +24063,13 @@
       </c>
       <c r="M19" s="155"/>
       <c r="N19" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>1.3.4 Rehabilitation - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>1.3.4 Rehabilitation - mapping to IUCN GET - 18</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:2.1.0</v>
       </c>
       <c r="B20" t="s">
@@ -24100,13 +24100,13 @@
         <v>1042</v>
       </c>
       <c r="N20" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>2.1.0 Grazing native vegetation - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>2.1.0 Grazing native vegetation - mapping to IUCN GET - 19</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:2.2.0</v>
       </c>
       <c r="B21" t="s">
@@ -24137,13 +24137,13 @@
         <v>1042</v>
       </c>
       <c r="N21" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>2.2.0 Production native forests - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>2.2.0 Production native forests - mapping to IUCN GET - 20</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:2.2.1</v>
       </c>
       <c r="B22" t="s">
@@ -24178,13 +24178,13 @@
       </c>
       <c r="M22" s="155"/>
       <c r="N22" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>2.2.1 Wood production forestry - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>2.2.1 Wood production forestry - mapping to IUCN GET - 21</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:2.2.2</v>
       </c>
       <c r="B23" t="s">
@@ -24219,13 +24219,13 @@
       </c>
       <c r="M23" s="155"/>
       <c r="N23" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>2.2.2 Other forest production - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>2.2.2 Other forest production - mapping to IUCN GET - 22</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.1.0</v>
       </c>
       <c r="B24" t="s">
@@ -24256,13 +24256,13 @@
         <v>1042</v>
       </c>
       <c r="N24" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.1.0 Plantation forests - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.1.0 Plantation forests - mapping to IUCN GET - 23</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.1.1</v>
       </c>
       <c r="B25" t="s">
@@ -24294,13 +24294,13 @@
       </c>
       <c r="M25" s="155"/>
       <c r="N25" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.1.1 Hardwood plantation forestry - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.1.1 Hardwood plantation forestry - mapping to IUCN GET - 24</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.1.2</v>
       </c>
       <c r="B26" t="s">
@@ -24332,13 +24332,13 @@
       </c>
       <c r="M26" s="155"/>
       <c r="N26" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.1.2 Softwood plantation forestry - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.1.2 Softwood plantation forestry - mapping to IUCN GET - 25</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.1.3</v>
       </c>
       <c r="B27" t="s">
@@ -24370,13 +24370,13 @@
       </c>
       <c r="M27" s="155"/>
       <c r="N27" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.1.3 Other forest plantation - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.1.3 Other forest plantation - mapping to IUCN GET - 26</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.1.4</v>
       </c>
       <c r="B28" t="s">
@@ -24408,13 +24408,13 @@
       </c>
       <c r="M28" s="155"/>
       <c r="N28" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.1.4 Environmental forest plantation - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.1.4 Environmental forest plantation - mapping to IUCN GET - 27</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.2.0</v>
       </c>
       <c r="B29" t="s">
@@ -24445,13 +24445,13 @@
         <v>1042</v>
       </c>
       <c r="N29" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.2.0 Grazing modified pastures - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.2.0 Grazing modified pastures - mapping to IUCN GET - 28</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.2.1</v>
       </c>
       <c r="B30" t="s">
@@ -24483,13 +24483,13 @@
       </c>
       <c r="M30" s="155"/>
       <c r="N30" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.2.1 Native/exotic pasture mosaic - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.2.1 Native/exotic pasture mosaic - mapping to IUCN GET - 29</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.2.2</v>
       </c>
       <c r="B31" s="17" t="s">
@@ -24521,13 +24521,13 @@
       </c>
       <c r="M31" s="155"/>
       <c r="N31" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.2.2 Woody fodder plants - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.2.2 Woody fodder plants - mapping to IUCN GET - 30</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.2.3</v>
       </c>
       <c r="B32" t="s">
@@ -24559,13 +24559,13 @@
       </c>
       <c r="M32" s="155"/>
       <c r="N32" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.2.3 Pasture legumes - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.2.3 Pasture legumes - mapping to IUCN GET - 31</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.2.4</v>
       </c>
       <c r="B33" t="s">
@@ -24597,13 +24597,13 @@
       </c>
       <c r="M33" s="155"/>
       <c r="N33" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.2.4 Pasture legume/grass mixtures - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.2.4 Pasture legume/grass mixtures - mapping to IUCN GET - 32</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.2.5</v>
       </c>
       <c r="B34" t="s">
@@ -24635,13 +24635,13 @@
       </c>
       <c r="M34" s="155"/>
       <c r="N34" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.2.5 Sown grasses - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.2.5 Sown grasses - mapping to IUCN GET - 33</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.3.0</v>
       </c>
       <c r="B35" t="s">
@@ -24672,13 +24672,13 @@
         <v>1042</v>
       </c>
       <c r="N35" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.3.0 Cropping - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.3.0 Cropping - mapping to IUCN GET - 34</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.3.1</v>
       </c>
       <c r="B36" t="s">
@@ -24710,13 +24710,13 @@
       </c>
       <c r="M36" s="155"/>
       <c r="N36" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.3.1 Cereals - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.3.1 Cereals - mapping to IUCN GET - 35</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.3.2</v>
       </c>
       <c r="B37" t="s">
@@ -24748,13 +24748,13 @@
       </c>
       <c r="M37" s="155"/>
       <c r="N37" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.3.2 Beverage and spice crops - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.3.2 Beverage and spice crops - mapping to IUCN GET - 36</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.3.3</v>
       </c>
       <c r="B38" t="s">
@@ -24786,13 +24786,13 @@
       </c>
       <c r="M38" s="155"/>
       <c r="N38" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.3.3 Hay and silage - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.3.3 Hay and silage - mapping to IUCN GET - 37</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.3.4</v>
       </c>
       <c r="B39" t="s">
@@ -24824,13 +24824,13 @@
       </c>
       <c r="M39" s="155"/>
       <c r="N39" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.3.4 Oilseeds - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.3.4 Oilseeds - mapping to IUCN GET - 38</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.3.5</v>
       </c>
       <c r="B40" t="s">
@@ -24862,13 +24862,13 @@
       </c>
       <c r="M40" s="155"/>
       <c r="N40" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.3.5 Sugar - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.3.5 Sugar - mapping to IUCN GET - 39</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.3.6</v>
       </c>
       <c r="B41" t="s">
@@ -24900,13 +24900,13 @@
       </c>
       <c r="M41" s="155"/>
       <c r="N41" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.3.6 Cotton - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.3.6 Cotton - mapping to IUCN GET - 40</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.3.7</v>
       </c>
       <c r="B42" t="s">
@@ -24938,13 +24938,13 @@
       </c>
       <c r="M42" s="155"/>
       <c r="N42" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.3.7 Alkaloid poppies - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.3.7 Alkaloid poppies - mapping to IUCN GET - 41</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.3.8</v>
       </c>
       <c r="B43" t="s">
@@ -24976,13 +24976,13 @@
       </c>
       <c r="M43" s="155"/>
       <c r="N43" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.3.8 Pulses - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.3.8 Pulses - mapping to IUCN GET - 42</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.4.0</v>
       </c>
       <c r="B44" t="s">
@@ -25013,13 +25013,13 @@
         <v>1042</v>
       </c>
       <c r="N44" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.4.0 Perennial horticulture - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.4.0 Perennial horticulture - mapping to IUCN GET - 43</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.4.1</v>
       </c>
       <c r="B45" t="s">
@@ -25051,13 +25051,13 @@
       </c>
       <c r="M45" s="155"/>
       <c r="N45" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.4.1 Tree fruits - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.4.1 Tree fruits - mapping to IUCN GET - 44</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.4.2</v>
       </c>
       <c r="B46" t="s">
@@ -25089,13 +25089,13 @@
       </c>
       <c r="M46" s="155"/>
       <c r="N46" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.4.2 Olives - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.4.2 Olives - mapping to IUCN GET - 45</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.4.3</v>
       </c>
       <c r="B47" t="s">
@@ -25127,13 +25127,13 @@
       </c>
       <c r="M47" s="155"/>
       <c r="N47" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.4.3 Tree nuts - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.4.3 Tree nuts - mapping to IUCN GET - 46</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.4.4</v>
       </c>
       <c r="B48" t="s">
@@ -25165,13 +25165,13 @@
       </c>
       <c r="M48" s="155"/>
       <c r="N48" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.4.4 Vine fruits - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.4.4 Vine fruits - mapping to IUCN GET - 47</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.4.5</v>
       </c>
       <c r="B49" t="s">
@@ -25203,13 +25203,13 @@
       </c>
       <c r="M49" s="155"/>
       <c r="N49" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.4.5 Shrub berries and fruits - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.4.5 Shrub berries and fruits - mapping to IUCN GET - 48</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.4.6</v>
       </c>
       <c r="B50" t="s">
@@ -25241,13 +25241,13 @@
       </c>
       <c r="M50" s="155"/>
       <c r="N50" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.4.6 Perennial flowers and bulbs - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.4.6 Perennial flowers and bulbs - mapping to IUCN GET - 49</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.4.7</v>
       </c>
       <c r="B51" t="s">
@@ -25279,13 +25279,13 @@
       </c>
       <c r="M51" s="155"/>
       <c r="N51" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.4.7 Perennial vegetables and herbs - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.4.7 Perennial vegetables and herbs - mapping to IUCN GET - 50</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.4.8</v>
       </c>
       <c r="B52" t="s">
@@ -25317,13 +25317,13 @@
       </c>
       <c r="M52" s="155"/>
       <c r="N52" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.4.8 Citrus - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.4.8 Citrus - mapping to IUCN GET - 51</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.4.9</v>
       </c>
       <c r="B53" t="s">
@@ -25355,13 +25355,13 @@
       </c>
       <c r="M53" s="155"/>
       <c r="N53" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.4.9 Grapes - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.4.9 Grapes - mapping to IUCN GET - 52</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.5.1</v>
       </c>
       <c r="B54" s="17" t="s">
@@ -25393,13 +25393,13 @@
       </c>
       <c r="M54" s="155"/>
       <c r="N54" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.5.1 Seasonal fruits - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.5.1 Seasonal fruits - mapping to IUCN GET - 53</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.5.2</v>
       </c>
       <c r="B55" t="s">
@@ -25431,13 +25431,13 @@
       </c>
       <c r="M55" s="155"/>
       <c r="N55" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.5.2 Seasonal flowers and bulbs - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.5.2 Seasonal flowers and bulbs - mapping to IUCN GET - 54</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.5.4</v>
       </c>
       <c r="B56" s="17" t="s">
@@ -25469,13 +25469,13 @@
       </c>
       <c r="M56" s="155"/>
       <c r="N56" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.5.4 Seasonal vegetables and herbs - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.5.4 Seasonal vegetables and herbs - mapping to IUCN GET - 55</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.6.1</v>
       </c>
       <c r="B57" t="s">
@@ -25510,13 +25510,13 @@
       </c>
       <c r="M57" s="155"/>
       <c r="N57" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.6.1 Degraded land - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.6.1 Degraded land - mapping to IUCN GET - 56</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.6.2</v>
       </c>
       <c r="B58" t="s">
@@ -25551,13 +25551,13 @@
       </c>
       <c r="M58" s="155"/>
       <c r="N58" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.6.2 Abandoned land - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.6.2 Abandoned land - mapping to IUCN GET - 57</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.6.3</v>
       </c>
       <c r="B59" t="s">
@@ -25592,13 +25592,13 @@
       </c>
       <c r="M59" s="155"/>
       <c r="N59" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.6.3 Land under rehabilitation - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.6.3 Land under rehabilitation - mapping to IUCN GET - 58</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.6.4</v>
       </c>
       <c r="B60" t="s">
@@ -25633,13 +25633,13 @@
       </c>
       <c r="M60" s="155"/>
       <c r="N60" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.6.4 No defined use - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.6.4 No defined use - mapping to IUCN GET - 59</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:3.6.5</v>
       </c>
       <c r="B61" t="s">
@@ -25674,13 +25674,13 @@
       </c>
       <c r="M61" s="155"/>
       <c r="N61" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>3.6.5 Abandoned perennial horticulture - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>3.6.5 Abandoned perennial horticulture - mapping to IUCN GET - 60</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:4.1.0</v>
       </c>
       <c r="B62" t="s">
@@ -25711,13 +25711,13 @@
         <v>1042</v>
       </c>
       <c r="N62" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>4.1.0 Irrigated plantation forests - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>4.1.0 Irrigated plantation forests - mapping to IUCN GET - 61</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:4.1.1</v>
       </c>
       <c r="B63" t="s">
@@ -25749,13 +25749,13 @@
       </c>
       <c r="M63" s="155"/>
       <c r="N63" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>4.1.1 Irrigated hardwood plantation forestry - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>4.1.1 Irrigated hardwood plantation forestry - mapping to IUCN GET - 62</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:4.1.2</v>
       </c>
       <c r="B64" t="s">
@@ -25787,13 +25787,13 @@
       </c>
       <c r="M64" s="155"/>
       <c r="N64" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>4.1.2 Irrigated softwood plantation forestry - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>4.1.2 Irrigated softwood plantation forestry - mapping to IUCN GET - 63</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:4.1.3</v>
       </c>
       <c r="B65" t="s">
@@ -25825,13 +25825,13 @@
       </c>
       <c r="M65" s="155"/>
       <c r="N65" s="155" t="str">
-        <f t="shared" si="0"/>
-        <v>4.1.3 Irrigated other forest production - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>4.1.3 Irrigated other forest production - mapping to IUCN GET - 64</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>alum:4.1.4</v>
       </c>
       <c r="B66" t="s">
@@ -25863,13 +25863,13 @@
       </c>
       <c r="M66" s="155"/>
       <c r="N66" s="155" t="str">
-        <f t="shared" ref="N66:N99" si="2">CONCATENATE(B66, " - mapping to IUCN GET")</f>
-        <v>4.1.4 Irrigated environmental forest plantation - mapping to IUCN GET</v>
+        <f t="shared" si="1"/>
+        <v>4.1.4 Irrigated environmental forest plantation - mapping to IUCN GET - 65</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" t="str">
-        <f t="shared" ref="A67:A130" si="3">_xlfn.CONCAT("alum:",LEFT(B67,FIND(" ",B67)-1))</f>
+        <f t="shared" ref="A67:A130" si="2">_xlfn.CONCAT("alum:",LEFT(B67,FIND(" ",B67)-1))</f>
         <v>alum:4.2.0</v>
       </c>
       <c r="B67" t="s">
@@ -25900,13 +25900,13 @@
         <v>1042</v>
       </c>
       <c r="N67" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.2.0 Grazing irrigated modified pastures - mapping to IUCN GET</v>
+        <f t="shared" ref="N67:N130" si="3">CONCATENATE(B67, " - mapping to IUCN GET - ", ROW(B67)-1)</f>
+        <v>4.2.0 Grazing irrigated modified pastures - mapping to IUCN GET - 66</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.2.1</v>
       </c>
       <c r="B68" t="s">
@@ -25938,13 +25938,13 @@
       </c>
       <c r="M68" s="155"/>
       <c r="N68" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.2.1 Irrigated woody fodder plants - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.2.1 Irrigated woody fodder plants - mapping to IUCN GET - 67</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.2.2</v>
       </c>
       <c r="B69" t="s">
@@ -25976,13 +25976,13 @@
       </c>
       <c r="M69" s="155"/>
       <c r="N69" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.2.2 Irrigated pasture legumes - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.2.2 Irrigated pasture legumes - mapping to IUCN GET - 68</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.2.3</v>
       </c>
       <c r="B70" t="s">
@@ -26014,13 +26014,13 @@
       </c>
       <c r="M70" s="155"/>
       <c r="N70" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.2.3 Irrigated legume/grass mixtures - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.2.3 Irrigated legume/grass mixtures - mapping to IUCN GET - 69</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.2.4</v>
       </c>
       <c r="B71" t="s">
@@ -26052,13 +26052,13 @@
       </c>
       <c r="M71" s="155"/>
       <c r="N71" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.2.4 Irrigated sown grasses - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.2.4 Irrigated sown grasses - mapping to IUCN GET - 70</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.3.0</v>
       </c>
       <c r="B72" t="s">
@@ -26089,13 +26089,13 @@
         <v>1042</v>
       </c>
       <c r="N72" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.3.0 Irrigated cropping - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.3.0 Irrigated cropping - mapping to IUCN GET - 71</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.3.1</v>
       </c>
       <c r="B73" t="s">
@@ -26127,13 +26127,13 @@
       </c>
       <c r="M73" s="155"/>
       <c r="N73" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.3.1 Irrigated cereals - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.3.1 Irrigated cereals - mapping to IUCN GET - 72</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.3.2</v>
       </c>
       <c r="B74" t="s">
@@ -26165,13 +26165,13 @@
       </c>
       <c r="M74" s="155"/>
       <c r="N74" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.3.2 Irrigated beverage and spice crops - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.3.2 Irrigated beverage and spice crops - mapping to IUCN GET - 73</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.3.3</v>
       </c>
       <c r="B75" t="s">
@@ -26203,13 +26203,13 @@
       </c>
       <c r="M75" s="155"/>
       <c r="N75" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.3.3 Irrigated hay and silage - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.3.3 Irrigated hay and silage - mapping to IUCN GET - 74</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.3.4</v>
       </c>
       <c r="B76" t="s">
@@ -26241,13 +26241,13 @@
       </c>
       <c r="M76" s="155"/>
       <c r="N76" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.3.4 Irrigated oilseeds - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.3.4 Irrigated oilseeds - mapping to IUCN GET - 75</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.3.5</v>
       </c>
       <c r="B77" t="s">
@@ -26279,13 +26279,13 @@
       </c>
       <c r="M77" s="155"/>
       <c r="N77" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.3.5 Irrigated sugar - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.3.5 Irrigated sugar - mapping to IUCN GET - 76</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.3.6</v>
       </c>
       <c r="B78" t="s">
@@ -26317,13 +26317,13 @@
       </c>
       <c r="M78" s="155"/>
       <c r="N78" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.3.6 Irrigated cotton - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.3.6 Irrigated cotton - mapping to IUCN GET - 77</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.3.7</v>
       </c>
       <c r="B79" t="s">
@@ -26355,13 +26355,13 @@
       </c>
       <c r="M79" s="155"/>
       <c r="N79" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.3.7 Irrigated alkaloid poppies - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.3.7 Irrigated alkaloid poppies - mapping to IUCN GET - 78</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.3.8</v>
       </c>
       <c r="B80" t="s">
@@ -26393,13 +26393,13 @@
       </c>
       <c r="M80" s="155"/>
       <c r="N80" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.3.8 Irrigated pulses - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.3.8 Irrigated pulses - mapping to IUCN GET - 79</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.3.9</v>
       </c>
       <c r="B81" t="s">
@@ -26431,13 +26431,13 @@
       </c>
       <c r="M81" s="155"/>
       <c r="N81" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.3.9 Irrigated rice - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.3.9 Irrigated rice - mapping to IUCN GET - 80</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.4.0</v>
       </c>
       <c r="B82" t="s">
@@ -26468,13 +26468,13 @@
         <v>1042</v>
       </c>
       <c r="N82" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.4.0 Irrigated perennial horticulture - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.4.0 Irrigated perennial horticulture - mapping to IUCN GET - 81</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.4.1</v>
       </c>
       <c r="B83" t="s">
@@ -26506,13 +26506,13 @@
       </c>
       <c r="M83" s="155"/>
       <c r="N83" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.4.1 Irrigated tree fruits - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.4.1 Irrigated tree fruits - mapping to IUCN GET - 82</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.4.2</v>
       </c>
       <c r="B84" t="s">
@@ -26544,13 +26544,13 @@
       </c>
       <c r="M84" s="155"/>
       <c r="N84" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.4.2 Irrigated olives - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.4.2 Irrigated olives - mapping to IUCN GET - 83</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.4.3</v>
       </c>
       <c r="B85" t="s">
@@ -26582,13 +26582,13 @@
       </c>
       <c r="M85" s="155"/>
       <c r="N85" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.4.3 Irrigated tree nuts - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.4.3 Irrigated tree nuts - mapping to IUCN GET - 84</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.4.4</v>
       </c>
       <c r="B86" t="s">
@@ -26620,13 +26620,13 @@
       </c>
       <c r="M86" s="155"/>
       <c r="N86" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.4.4 Irrigated vine fruits - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.4.4 Irrigated vine fruits - mapping to IUCN GET - 85</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.4.5</v>
       </c>
       <c r="B87" t="s">
@@ -26658,13 +26658,13 @@
       </c>
       <c r="M87" s="155"/>
       <c r="N87" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.4.5 Irrigated shrub berries and fruits - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.4.5 Irrigated shrub berries and fruits - mapping to IUCN GET - 86</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.4.6</v>
       </c>
       <c r="B88" t="s">
@@ -26696,13 +26696,13 @@
       </c>
       <c r="M88" s="155"/>
       <c r="N88" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.4.6 Irrigated  perennial flowers and bulbs - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.4.6 Irrigated  perennial flowers and bulbs - mapping to IUCN GET - 87</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.4.7</v>
       </c>
       <c r="B89" t="s">
@@ -26734,13 +26734,13 @@
       </c>
       <c r="M89" s="155"/>
       <c r="N89" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.4.7 Irrigated perennial vegetables and herbs - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.4.7 Irrigated perennial vegetables and herbs - mapping to IUCN GET - 88</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.4.8</v>
       </c>
       <c r="B90" t="s">
@@ -26772,13 +26772,13 @@
       </c>
       <c r="M90" s="155"/>
       <c r="N90" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.4.8 Irrigated citrus - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.4.8 Irrigated citrus - mapping to IUCN GET - 89</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.4.9</v>
       </c>
       <c r="B91" t="s">
@@ -26810,13 +26810,13 @@
       </c>
       <c r="M91" s="155"/>
       <c r="N91" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.4.9 Irrigated grapes - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.4.9 Irrigated grapes - mapping to IUCN GET - 90</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.5.1</v>
       </c>
       <c r="B92" s="17" t="s">
@@ -26848,13 +26848,13 @@
       </c>
       <c r="M92" s="155"/>
       <c r="N92" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.5.1 Irrigated seasonal fruits - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.5.1 Irrigated seasonal fruits - mapping to IUCN GET - 91</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.5.2</v>
       </c>
       <c r="B93" t="s">
@@ -26886,13 +26886,13 @@
       </c>
       <c r="M93" s="155"/>
       <c r="N93" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.5.2 Irrigated seasonal flowers and bulbs - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.5.2 Irrigated seasonal flowers and bulbs - mapping to IUCN GET - 92</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.5.3</v>
       </c>
       <c r="B94" t="s">
@@ -26924,13 +26924,13 @@
       </c>
       <c r="M94" s="155"/>
       <c r="N94" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.5.3 Irrigated seasonal vegetables and herbs - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.5.3 Irrigated seasonal vegetables and herbs - mapping to IUCN GET - 93</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.5.4</v>
       </c>
       <c r="B95" t="s">
@@ -26962,13 +26962,13 @@
       </c>
       <c r="M95" s="155"/>
       <c r="N95" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.5.4 Irrigated turf farming - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.5.4 Irrigated turf farming - mapping to IUCN GET - 94</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.6.1</v>
       </c>
       <c r="B96" t="s">
@@ -27003,13 +27003,13 @@
       </c>
       <c r="M96" s="155"/>
       <c r="N96" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.6.1 Degraded irrigated land - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.6.1 Degraded irrigated land - mapping to IUCN GET - 95</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.6.2</v>
       </c>
       <c r="B97" t="s">
@@ -27044,13 +27044,13 @@
       </c>
       <c r="M97" s="155"/>
       <c r="N97" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.6.2 Abandoned irrigated land - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.6.2 Abandoned irrigated land - mapping to IUCN GET - 96</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.6.3</v>
       </c>
       <c r="B98" t="s">
@@ -27085,13 +27085,13 @@
       </c>
       <c r="M98" s="155"/>
       <c r="N98" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.6.3 Irrigated land under rehabilitation - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.6.3 Irrigated land under rehabilitation - mapping to IUCN GET - 97</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.6.4</v>
       </c>
       <c r="B99" t="s">
@@ -27126,13 +27126,13 @@
       </c>
       <c r="M99" s="155"/>
       <c r="N99" s="155" t="str">
-        <f t="shared" si="2"/>
-        <v>4.6.4 No defined use - irrigation - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.6.4 No defined use - irrigation - mapping to IUCN GET - 98</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:4.6.5</v>
       </c>
       <c r="B100" t="s">
@@ -27167,13 +27167,13 @@
       </c>
       <c r="M100" s="155"/>
       <c r="N100" s="155" t="str">
-        <f>CONCATENATE(B100, " - mapping to IUCN GET")</f>
-        <v>4.6.5 Abandoned irrigated perennial horticulture - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>4.6.5 Abandoned irrigated perennial horticulture - mapping to IUCN GET - 99</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.0.0</v>
       </c>
       <c r="B101" s="17" t="s">
@@ -27205,13 +27205,13 @@
       </c>
       <c r="M101" s="155"/>
       <c r="N101" s="155" t="str">
-        <f t="shared" ref="N101:N164" si="4">CONCATENATE(B101, " - mapping to IUCN GET")</f>
-        <v>5.0.0 Intensive uses - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.0.0 Intensive uses - mapping to IUCN GET - 100</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.1.0</v>
       </c>
       <c r="B102" t="s">
@@ -27242,13 +27242,13 @@
         <v>1042</v>
       </c>
       <c r="N102" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.1.0 Intensive horticulture - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.1.0 Intensive horticulture - mapping to IUCN GET - 101</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.1.1</v>
       </c>
       <c r="B103" t="s">
@@ -27280,13 +27280,13 @@
       </c>
       <c r="M103" s="155"/>
       <c r="N103" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.1.1 Production nurseries - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.1.1 Production nurseries - mapping to IUCN GET - 102</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.1.2</v>
       </c>
       <c r="B104" t="s">
@@ -27318,13 +27318,13 @@
       </c>
       <c r="M104" s="155"/>
       <c r="N104" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.1.2 Shadehouses - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.1.2 Shadehouses - mapping to IUCN GET - 103</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.1.3</v>
       </c>
       <c r="B105" t="s">
@@ -27356,13 +27356,13 @@
       </c>
       <c r="M105" s="155"/>
       <c r="N105" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.1.3 Glasshouses - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.1.3 Glasshouses - mapping to IUCN GET - 104</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.1.4</v>
       </c>
       <c r="B106" t="s">
@@ -27394,13 +27394,13 @@
       </c>
       <c r="M106" s="155"/>
       <c r="N106" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.1.4 Glasshouses (hydroponic) - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.1.4 Glasshouses (hydroponic) - mapping to IUCN GET - 105</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.1.5</v>
       </c>
       <c r="B107" t="s">
@@ -27432,13 +27432,13 @@
       </c>
       <c r="M107" s="155"/>
       <c r="N107" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.1.5 Abandoned intensive horticulture - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.1.5 Abandoned intensive horticulture - mapping to IUCN GET - 106</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.2.0</v>
       </c>
       <c r="B108" t="s">
@@ -27469,13 +27469,13 @@
         <v>1042</v>
       </c>
       <c r="N108" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.2.0 Intensive animal production - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.2.0 Intensive animal production - mapping to IUCN GET - 107</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.2.1</v>
       </c>
       <c r="B109" t="s">
@@ -27507,13 +27507,13 @@
       </c>
       <c r="M109" s="155"/>
       <c r="N109" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.2.1 Dairy sheds and yards - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.2.1 Dairy sheds and yards - mapping to IUCN GET - 108</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.2.2</v>
       </c>
       <c r="B110" t="s">
@@ -27545,13 +27545,13 @@
       </c>
       <c r="M110" s="155"/>
       <c r="N110" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.2.2 Feedlots - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.2.2 Feedlots - mapping to IUCN GET - 109</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.2.3</v>
       </c>
       <c r="B111" t="s">
@@ -27583,13 +27583,13 @@
       </c>
       <c r="M111" s="155"/>
       <c r="N111" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.2.3 Poultry farms - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.2.3 Poultry farms - mapping to IUCN GET - 110</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.2.4</v>
       </c>
       <c r="B112" t="s">
@@ -27621,13 +27621,13 @@
       </c>
       <c r="M112" s="155"/>
       <c r="N112" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.2.4 Piggeries - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.2.4 Piggeries - mapping to IUCN GET - 111</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.2.5</v>
       </c>
       <c r="B113" t="s">
@@ -27659,13 +27659,13 @@
       </c>
       <c r="M113" s="155"/>
       <c r="N113" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.2.5 Aquaculture - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.2.5 Aquaculture - mapping to IUCN GET - 112</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.2.6</v>
       </c>
       <c r="B114" t="s">
@@ -27697,13 +27697,13 @@
       </c>
       <c r="M114" s="155"/>
       <c r="N114" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.2.6 Horse studs - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.2.6 Horse studs - mapping to IUCN GET - 113</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.2.7</v>
       </c>
       <c r="B115" t="s">
@@ -27735,13 +27735,13 @@
       </c>
       <c r="M115" s="155"/>
       <c r="N115" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.2.7 Saleyards/stockyards - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.2.7 Saleyards/stockyards - mapping to IUCN GET - 114</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.2.8</v>
       </c>
       <c r="B116" t="s">
@@ -27773,13 +27773,13 @@
       </c>
       <c r="M116" s="155"/>
       <c r="N116" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.2.8 Abandoned intensive animal production - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.2.8 Abandoned intensive animal production - mapping to IUCN GET - 115</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.3.0</v>
       </c>
       <c r="B117" t="s">
@@ -27810,13 +27810,13 @@
         <v>1042</v>
       </c>
       <c r="N117" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.3.0 Manufacturing and industrial - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.3.0 Manufacturing and industrial - mapping to IUCN GET - 116</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.3.1</v>
       </c>
       <c r="B118" t="s">
@@ -27848,13 +27848,13 @@
       </c>
       <c r="M118" s="155"/>
       <c r="N118" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.3.1 General purpose factory - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.3.1 General purpose factory - mapping to IUCN GET - 117</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.3.2</v>
       </c>
       <c r="B119" t="s">
@@ -27886,13 +27886,13 @@
       </c>
       <c r="M119" s="155"/>
       <c r="N119" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.3.2 Food processing factory - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.3.2 Food processing factory - mapping to IUCN GET - 118</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.3.3</v>
       </c>
       <c r="B120" t="s">
@@ -27924,13 +27924,13 @@
       </c>
       <c r="M120" s="155"/>
       <c r="N120" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.3.3 Major industrial complex - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.3.3 Major industrial complex - mapping to IUCN GET - 119</v>
       </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.3.4</v>
       </c>
       <c r="B121" t="s">
@@ -27962,13 +27962,13 @@
       </c>
       <c r="M121" s="155"/>
       <c r="N121" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.3.4 Bulk grain storage - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.3.4 Bulk grain storage - mapping to IUCN GET - 120</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.3.5</v>
       </c>
       <c r="B122" t="s">
@@ -28000,13 +28000,13 @@
       </c>
       <c r="M122" s="155"/>
       <c r="N122" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.3.5 Abattoirs - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.3.5 Abattoirs - mapping to IUCN GET - 121</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.3.6</v>
       </c>
       <c r="B123" t="s">
@@ -28038,13 +28038,13 @@
       </c>
       <c r="M123" s="155"/>
       <c r="N123" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.3.6 Oil refinery - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.3.6 Oil refinery - mapping to IUCN GET - 122</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.3.7</v>
       </c>
       <c r="B124" t="s">
@@ -28076,13 +28076,13 @@
       </c>
       <c r="M124" s="155"/>
       <c r="N124" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.3.7 Sawmill - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.3.7 Sawmill - mapping to IUCN GET - 123</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.3.8</v>
       </c>
       <c r="B125" t="s">
@@ -28114,13 +28114,13 @@
       </c>
       <c r="M125" s="155"/>
       <c r="N125" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.3.8 Abandoned manufacturing and industrial - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.3.8 Abandoned manufacturing and industrial - mapping to IUCN GET - 124</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.4.0</v>
       </c>
       <c r="B126" t="s">
@@ -28151,13 +28151,13 @@
         <v>1042</v>
       </c>
       <c r="N126" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.4.0 Residential and farm infrastructure - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.4.0 Residential and farm infrastructure - mapping to IUCN GET - 125</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.4.1</v>
       </c>
       <c r="B127" t="s">
@@ -28189,13 +28189,13 @@
       </c>
       <c r="M127" s="155"/>
       <c r="N127" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.4.1 Urban residential - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.4.1 Urban residential - mapping to IUCN GET - 126</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.4.2</v>
       </c>
       <c r="B128" t="s">
@@ -28227,13 +28227,13 @@
       </c>
       <c r="M128" s="155"/>
       <c r="N128" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.4.2 Rural residential with agriculture - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.4.2 Rural residential with agriculture - mapping to IUCN GET - 127</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.4.3</v>
       </c>
       <c r="B129" t="s">
@@ -28265,13 +28265,13 @@
       </c>
       <c r="M129" s="155"/>
       <c r="N129" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.4.3 Rural residential without agriculture - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.4.3 Rural residential without agriculture - mapping to IUCN GET - 128</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>alum:5.4.4</v>
       </c>
       <c r="B130" t="s">
@@ -28303,13 +28303,13 @@
       </c>
       <c r="M130" s="155"/>
       <c r="N130" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.4.4 Remote communities - mapping to IUCN GET</v>
+        <f t="shared" si="3"/>
+        <v>5.4.4 Remote communities - mapping to IUCN GET - 129</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A131" t="str">
-        <f t="shared" ref="A131:A189" si="5">_xlfn.CONCAT("alum:",LEFT(B131,FIND(" ",B131)-1))</f>
+        <f t="shared" ref="A131:A189" si="4">_xlfn.CONCAT("alum:",LEFT(B131,FIND(" ",B131)-1))</f>
         <v>alum:5.4.5</v>
       </c>
       <c r="B131" t="s">
@@ -28341,13 +28341,13 @@
       </c>
       <c r="M131" s="155"/>
       <c r="N131" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.4.5 Farm buildings/infrastructure - mapping to IUCN GET</v>
+        <f t="shared" ref="N131:N189" si="5">CONCATENATE(B131, " - mapping to IUCN GET - ", ROW(B131)-1)</f>
+        <v>5.4.5 Farm buildings/infrastructure - mapping to IUCN GET - 130</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.5.0</v>
       </c>
       <c r="B132" t="s">
@@ -28378,13 +28378,13 @@
         <v>1042</v>
       </c>
       <c r="N132" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.5.0 Services - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.5.0 Services - mapping to IUCN GET - 131</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A133" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.5.1</v>
       </c>
       <c r="B133" t="s">
@@ -28416,13 +28416,13 @@
       </c>
       <c r="M133" s="155"/>
       <c r="N133" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.5.1 Commercial services - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.5.1 Commercial services - mapping to IUCN GET - 132</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.5.2</v>
       </c>
       <c r="B134" t="s">
@@ -28454,13 +28454,13 @@
       </c>
       <c r="M134" s="155"/>
       <c r="N134" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.5.2 Public services - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.5.2 Public services - mapping to IUCN GET - 133</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.5.3</v>
       </c>
       <c r="B135" t="s">
@@ -28492,13 +28492,13 @@
       </c>
       <c r="M135" s="155"/>
       <c r="N135" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.5.3 Recreation and culture - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.5.3 Recreation and culture - mapping to IUCN GET - 134</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.5.4</v>
       </c>
       <c r="B136" t="s">
@@ -28530,13 +28530,13 @@
       </c>
       <c r="M136" s="155"/>
       <c r="N136" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.5.4 Defence facilities - urban - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.5.4 Defence facilities - urban - mapping to IUCN GET - 135</v>
       </c>
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.5.5</v>
       </c>
       <c r="B137" t="s">
@@ -28568,13 +28568,13 @@
       </c>
       <c r="M137" s="155"/>
       <c r="N137" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.5.5 Research facilities - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.5.5 Research facilities - mapping to IUCN GET - 136</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.6.0</v>
       </c>
       <c r="B138" t="s">
@@ -28605,13 +28605,13 @@
         <v>1042</v>
       </c>
       <c r="N138" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.6.0 Utilities - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.6.0 Utilities - mapping to IUCN GET - 137</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.6.1</v>
       </c>
       <c r="B139" t="s">
@@ -28643,13 +28643,13 @@
       </c>
       <c r="M139" s="155"/>
       <c r="N139" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.6.1 Fuel powered electricity generation - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.6.1 Fuel powered electricity generation - mapping to IUCN GET - 138</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.6.2</v>
       </c>
       <c r="B140" t="s">
@@ -28681,13 +28681,13 @@
       </c>
       <c r="M140" s="155"/>
       <c r="N140" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.6.2 Hydro electricity generation - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.6.2 Hydro electricity generation - mapping to IUCN GET - 139</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.6.3</v>
       </c>
       <c r="B141" t="s">
@@ -28719,13 +28719,13 @@
       </c>
       <c r="M141" s="155"/>
       <c r="N141" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.6.3 Wind electricity generation - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.6.3 Wind electricity generation - mapping to IUCN GET - 140</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.6.4</v>
       </c>
       <c r="B142" t="s">
@@ -28757,13 +28757,13 @@
       </c>
       <c r="M142" s="155"/>
       <c r="N142" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.6.4 Solar electricity generation - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.6.4 Solar electricity generation - mapping to IUCN GET - 141</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.6.5</v>
       </c>
       <c r="B143" t="s">
@@ -28795,13 +28795,13 @@
       </c>
       <c r="M143" s="155"/>
       <c r="N143" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.6.5 Electricity substations and transmission - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.6.5 Electricity substations and transmission - mapping to IUCN GET - 142</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.6.6</v>
       </c>
       <c r="B144" t="s">
@@ -28833,13 +28833,13 @@
       </c>
       <c r="M144" s="155"/>
       <c r="N144" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.6.6 Gas treatment, storage and transmission - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.6.6 Gas treatment, storage and transmission - mapping to IUCN GET - 143</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.6.7</v>
       </c>
       <c r="B145" t="s">
@@ -28871,13 +28871,13 @@
       </c>
       <c r="M145" s="155"/>
       <c r="N145" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.6.7 Water extraction and transmission - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.6.7 Water extraction and transmission - mapping to IUCN GET - 144</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.7.0</v>
       </c>
       <c r="B146" t="s">
@@ -28908,13 +28908,13 @@
         <v>1042</v>
       </c>
       <c r="N146" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.7.0 Transport and communication - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.7.0 Transport and communication - mapping to IUCN GET - 145</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.7.1</v>
       </c>
       <c r="B147" t="s">
@@ -28946,13 +28946,13 @@
       </c>
       <c r="M147" s="155"/>
       <c r="N147" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.7.1 Airports/aerodromes - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.7.1 Airports/aerodromes - mapping to IUCN GET - 146</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.7.2</v>
       </c>
       <c r="B148" t="s">
@@ -28984,13 +28984,13 @@
       </c>
       <c r="M148" s="155"/>
       <c r="N148" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.7.2 Roads - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.7.2 Roads - mapping to IUCN GET - 147</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A149" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.7.3</v>
       </c>
       <c r="B149" t="s">
@@ -29022,13 +29022,13 @@
       </c>
       <c r="M149" s="155"/>
       <c r="N149" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.7.3 Railways - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.7.3 Railways - mapping to IUCN GET - 148</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.7.4</v>
       </c>
       <c r="B150" t="s">
@@ -29060,13 +29060,13 @@
       </c>
       <c r="M150" s="155"/>
       <c r="N150" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.7.4 Ports and water transport - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.7.4 Ports and water transport - mapping to IUCN GET - 149</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A151" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.7.5</v>
       </c>
       <c r="B151" t="s">
@@ -29098,13 +29098,13 @@
       </c>
       <c r="M151" s="155"/>
       <c r="N151" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.7.5 Navigation and communication - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.7.5 Navigation and communication - mapping to IUCN GET - 150</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A152" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.8.0</v>
       </c>
       <c r="B152" t="s">
@@ -29135,13 +29135,13 @@
         <v>1042</v>
       </c>
       <c r="N152" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.8.0 Mining - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.8.0 Mining - mapping to IUCN GET - 151</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A153" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.8.1</v>
       </c>
       <c r="B153" t="s">
@@ -29173,13 +29173,13 @@
       </c>
       <c r="M153" s="155"/>
       <c r="N153" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.8.1 Mines - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.8.1 Mines - mapping to IUCN GET - 152</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A154" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.8.2</v>
       </c>
       <c r="B154" t="s">
@@ -29211,13 +29211,13 @@
       </c>
       <c r="M154" s="155"/>
       <c r="N154" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.8.2 Quarries - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.8.2 Quarries - mapping to IUCN GET - 153</v>
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A155" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.8.3</v>
       </c>
       <c r="B155" t="s">
@@ -29249,13 +29249,13 @@
       </c>
       <c r="M155" s="155"/>
       <c r="N155" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.8.3 Tailings - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.8.3 Tailings - mapping to IUCN GET - 154</v>
       </c>
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A156" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.8.4</v>
       </c>
       <c r="B156" t="s">
@@ -29287,13 +29287,13 @@
       </c>
       <c r="M156" s="155"/>
       <c r="N156" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.8.4 Extractive industry not in use - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.8.4 Extractive industry not in use - mapping to IUCN GET - 155</v>
       </c>
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A157" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.9.0</v>
       </c>
       <c r="B157" t="s">
@@ -29324,13 +29324,13 @@
         <v>1042</v>
       </c>
       <c r="N157" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.9.0 Waste treatment and disposal - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.9.0 Waste treatment and disposal - mapping to IUCN GET - 156</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A158" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.9.1</v>
       </c>
       <c r="B158" t="s">
@@ -29362,13 +29362,13 @@
       </c>
       <c r="M158" s="155"/>
       <c r="N158" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.9.1 Effluent pond - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.9.1 Effluent pond - mapping to IUCN GET - 157</v>
       </c>
     </row>
     <row r="159" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A159" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.9.2</v>
       </c>
       <c r="B159" t="s">
@@ -29400,13 +29400,13 @@
       </c>
       <c r="M159" s="155"/>
       <c r="N159" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.9.2 Landfill - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.9.2 Landfill - mapping to IUCN GET - 158</v>
       </c>
     </row>
     <row r="160" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A160" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.9.3</v>
       </c>
       <c r="B160" t="s">
@@ -29438,13 +29438,13 @@
       </c>
       <c r="M160" s="155"/>
       <c r="N160" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.9.3 Solid garbage - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.9.3 Solid garbage - mapping to IUCN GET - 159</v>
       </c>
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A161" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.9.4</v>
       </c>
       <c r="B161" t="s">
@@ -29476,13 +29476,13 @@
       </c>
       <c r="M161" s="155"/>
       <c r="N161" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.9.4 Incinerators - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.9.4 Incinerators - mapping to IUCN GET - 160</v>
       </c>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:5.9.5</v>
       </c>
       <c r="B162" t="s">
@@ -29514,13 +29514,13 @@
       </c>
       <c r="M162" s="155"/>
       <c r="N162" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>5.9.5 Sewage/sewerage - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>5.9.5 Sewage/sewerage - mapping to IUCN GET - 161</v>
       </c>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A163" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.0.0</v>
       </c>
       <c r="B163" t="s">
@@ -29551,13 +29551,13 @@
         <v>1042</v>
       </c>
       <c r="N163" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>6.0.0 Water - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.0.0 Water - mapping to IUCN GET - 162</v>
       </c>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A164" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.1.0</v>
       </c>
       <c r="B164" t="s">
@@ -29588,13 +29588,13 @@
         <v>1042</v>
       </c>
       <c r="N164" s="155" t="str">
-        <f t="shared" si="4"/>
-        <v>6.1.0 Lake - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.1.0 Lake - mapping to IUCN GET - 163</v>
       </c>
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A165" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.1.1</v>
       </c>
       <c r="B165" t="s">
@@ -29629,13 +29629,13 @@
       </c>
       <c r="M165" s="155"/>
       <c r="N165" s="155" t="str">
-        <f t="shared" ref="N165:N189" si="6">CONCATENATE(B165, " - mapping to IUCN GET")</f>
-        <v>6.1.1 Lake - conservation - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.1.1 Lake - conservation - mapping to IUCN GET - 164</v>
       </c>
     </row>
     <row r="166" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A166" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.1.2</v>
       </c>
       <c r="B166" t="s">
@@ -29670,13 +29670,13 @@
       </c>
       <c r="M166" s="155"/>
       <c r="N166" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.1.2 Lake - production - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.1.2 Lake - production - mapping to IUCN GET - 165</v>
       </c>
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A167" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.1.3</v>
       </c>
       <c r="B167" t="s">
@@ -29711,13 +29711,13 @@
       </c>
       <c r="M167" s="155"/>
       <c r="N167" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.1.3 Lake - intensive use - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.1.3 Lake - intensive use - mapping to IUCN GET - 166</v>
       </c>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A168" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.1.4</v>
       </c>
       <c r="B168" t="s">
@@ -29749,13 +29749,13 @@
       </c>
       <c r="M168" s="155"/>
       <c r="N168" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.1.4 Lake - saline - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.1.4 Lake - saline - mapping to IUCN GET - 167</v>
       </c>
     </row>
     <row r="169" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A169" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.2.0</v>
       </c>
       <c r="B169" t="s">
@@ -29786,13 +29786,13 @@
         <v>1042</v>
       </c>
       <c r="N169" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.2.0 Reservoir/dam - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.2.0 Reservoir/dam - mapping to IUCN GET - 168</v>
       </c>
     </row>
     <row r="170" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A170" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.2.1</v>
       </c>
       <c r="B170" t="s">
@@ -29824,13 +29824,13 @@
       </c>
       <c r="M170" s="155"/>
       <c r="N170" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.2.1 Reservoir - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.2.1 Reservoir - mapping to IUCN GET - 169</v>
       </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A171" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.2.2</v>
       </c>
       <c r="B171" t="s">
@@ -29862,13 +29862,13 @@
       </c>
       <c r="M171" s="155"/>
       <c r="N171" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.2.2 Water storage - intensive use/farm dams - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.2.2 Water storage - intensive use/farm dams - mapping to IUCN GET - 170</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A172" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.2.3</v>
       </c>
       <c r="B172" t="s">
@@ -29900,13 +29900,13 @@
       </c>
       <c r="M172" s="155"/>
       <c r="N172" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.2.3 Evaporation basin - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.2.3 Evaporation basin - mapping to IUCN GET - 171</v>
       </c>
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A173" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.3.0</v>
       </c>
       <c r="B173" t="s">
@@ -29937,13 +29937,13 @@
         <v>1042</v>
       </c>
       <c r="N173" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.3.0 River - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.3.0 River - mapping to IUCN GET - 172</v>
       </c>
     </row>
     <row r="174" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A174" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.3.1</v>
       </c>
       <c r="B174" t="s">
@@ -29978,13 +29978,13 @@
       </c>
       <c r="M174" s="155"/>
       <c r="N174" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.3.1 River - conservation - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.3.1 River - conservation - mapping to IUCN GET - 173</v>
       </c>
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A175" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.3.2</v>
       </c>
       <c r="B175" t="s">
@@ -30019,13 +30019,13 @@
       </c>
       <c r="M175" s="155"/>
       <c r="N175" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.3.2 River - production - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.3.2 River - production - mapping to IUCN GET - 174</v>
       </c>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A176" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.3.3</v>
       </c>
       <c r="B176" t="s">
@@ -30060,13 +30060,13 @@
       </c>
       <c r="M176" s="155"/>
       <c r="N176" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.3.3 River - intensive use - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.3.3 River - intensive use - mapping to IUCN GET - 175</v>
       </c>
     </row>
     <row r="177" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A177" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.4.0</v>
       </c>
       <c r="B177" t="s">
@@ -30097,13 +30097,13 @@
         <v>1042</v>
       </c>
       <c r="N177" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.4.0 Channel/aqueduct - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.4.0 Channel/aqueduct - mapping to IUCN GET - 176</v>
       </c>
     </row>
     <row r="178" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A178" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.4.1</v>
       </c>
       <c r="B178" t="s">
@@ -30135,13 +30135,13 @@
       </c>
       <c r="M178" s="155"/>
       <c r="N178" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.4.1 Supply channel/aqueduct - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.4.1 Supply channel/aqueduct - mapping to IUCN GET - 177</v>
       </c>
     </row>
     <row r="179" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A179" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.4.2</v>
       </c>
       <c r="B179" t="s">
@@ -30173,13 +30173,13 @@
       </c>
       <c r="M179" s="155"/>
       <c r="N179" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.4.2 Drainage channel/aqueduct - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.4.2 Drainage channel/aqueduct - mapping to IUCN GET - 178</v>
       </c>
     </row>
     <row r="180" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A180" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.4.3</v>
       </c>
       <c r="B180" t="s">
@@ -30211,13 +30211,13 @@
       </c>
       <c r="M180" s="155"/>
       <c r="N180" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.4.3 Stormwater - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.4.3 Stormwater - mapping to IUCN GET - 179</v>
       </c>
     </row>
     <row r="181" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A181" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.5.0</v>
       </c>
       <c r="B181" t="s">
@@ -30248,13 +30248,13 @@
         <v>1042</v>
       </c>
       <c r="N181" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.5.0 Marsh/wetland - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.5.0 Marsh/wetland - mapping to IUCN GET - 180</v>
       </c>
     </row>
     <row r="182" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A182" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.5.1</v>
       </c>
       <c r="B182" t="s">
@@ -30289,13 +30289,13 @@
       </c>
       <c r="M182" s="155"/>
       <c r="N182" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.5.1 Marsh/wetland - conservation - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.5.1 Marsh/wetland - conservation - mapping to IUCN GET - 181</v>
       </c>
     </row>
     <row r="183" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A183" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.5.2</v>
       </c>
       <c r="B183" t="s">
@@ -30330,13 +30330,13 @@
       </c>
       <c r="M183" s="155"/>
       <c r="N183" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.5.2 Marsh/wetland - production - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.5.2 Marsh/wetland - production - mapping to IUCN GET - 182</v>
       </c>
     </row>
     <row r="184" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A184" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.5.3</v>
       </c>
       <c r="B184" t="s">
@@ -30371,13 +30371,13 @@
       </c>
       <c r="M184" s="155"/>
       <c r="N184" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.5.3 Marsh/wetland - intensive use - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.5.3 Marsh/wetland - intensive use - mapping to IUCN GET - 183</v>
       </c>
     </row>
     <row r="185" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A185" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.5.4</v>
       </c>
       <c r="B185" t="s">
@@ -30409,13 +30409,13 @@
       </c>
       <c r="M185" s="155"/>
       <c r="N185" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.5.4 Marsh/wetland - saline - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.5.4 Marsh/wetland - saline - mapping to IUCN GET - 184</v>
       </c>
     </row>
     <row r="186" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A186" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.6.0</v>
       </c>
       <c r="B186" t="s">
@@ -30446,13 +30446,13 @@
         <v>1042</v>
       </c>
       <c r="N186" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.6.0 Estuary/coastal waters - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.6.0 Estuary/coastal waters - mapping to IUCN GET - 185</v>
       </c>
     </row>
     <row r="187" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A187" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.6.1</v>
       </c>
       <c r="B187" t="s">
@@ -30487,13 +30487,13 @@
       </c>
       <c r="M187" s="155"/>
       <c r="N187" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.6.1 Estuary/coastal waters - conservation - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.6.1 Estuary/coastal waters - conservation - mapping to IUCN GET - 186</v>
       </c>
     </row>
     <row r="188" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A188" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.6.2</v>
       </c>
       <c r="B188" t="s">
@@ -30528,13 +30528,13 @@
       </c>
       <c r="M188" s="155"/>
       <c r="N188" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.6.2 Estuary/coastal waters - production - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.6.2 Estuary/coastal waters - production - mapping to IUCN GET - 187</v>
       </c>
     </row>
     <row r="189" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A189" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>alum:6.6.3</v>
       </c>
       <c r="B189" t="s">
@@ -30569,8 +30569,8 @@
       </c>
       <c r="M189" s="155"/>
       <c r="N189" s="155" t="str">
-        <f t="shared" si="6"/>
-        <v>6.6.3 Estuary/coastal waters - intensive use - mapping to IUCN GET</v>
+        <f t="shared" si="5"/>
+        <v>6.6.3 Estuary/coastal waters - intensive use - mapping to IUCN GET - 188</v>
       </c>
     </row>
   </sheetData>
@@ -30627,15 +30627,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC29B5BE6945C34F8C7CB81794666E31" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f7151ef105987b2d3758ef53560e213">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48c5b5cd9b8d25ff6dd15848836f4270" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -30767,6 +30758,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
   <ds:schemaRefs>
@@ -30778,14 +30778,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97EDE51C-194A-4D85-AD03-32004056A6AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30801,4 +30793,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added simple lists of unique EFGS to sheet in crosswalks
</commit_message>
<xml_diff>
--- a/crosswalks/ALUM-IUCNGET/ALUM-IUCNGET.xlsx
+++ b/crosswalks/ALUM-IUCNGET/ALUM-IUCNGET.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94CE728B-2C81-44C7-A9F4-650A7F52181D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D49348-DC96-4662-A79B-08A9172DE033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="9660" windowWidth="34230" windowHeight="10815" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALUM V8" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="header" sheetId="15" r:id="rId8"/>
     <sheet name="SSSOM" sheetId="14" r:id="rId9"/>
     <sheet name="CHANGE_LOG" sheetId="16" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="18" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">commodities!$A$2:$F$268</definedName>
@@ -33,20 +34,7 @@
     <definedName name="Z_AB65B437_1B49_4040_B070_7D10DCCE9FB5_.wvu.PrintArea" localSheetId="0" hidden="1">'ALUM V8'!$A$1:$S$75</definedName>
     <definedName name="Z_E13C975D_9911_46DF_BB53_0E45A3160659_.wvu.PrintArea" localSheetId="0" hidden="1">'ALUM V8'!$A$1:$S$77</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -75,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5435" uniqueCount="1304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5444" uniqueCount="1304">
   <si>
     <t>Perennial horticulture</t>
   </si>
@@ -8440,6 +8428,72 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CA0BFD-6560-4468-8D95-F8BDB1DE431A}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A9">
+    <sortCondition ref="A1:A9"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2">
@@ -23271,9 +23325,9 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:N189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24:E185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -30618,12 +30672,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -30759,20 +30813,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -30796,9 +30848,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
6.2.2 Water storage - intensive use/farm dams has been remapped to F3.2 Constructed lacustrine wetlands.
</commit_message>
<xml_diff>
--- a/crosswalks/ALUM-IUCNGET/ALUM-IUCNGET.xlsx
+++ b/crosswalks/ALUM-IUCNGET/ALUM-IUCNGET.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D49348-DC96-4662-A79B-08A9172DE033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60C02F5-ED80-4721-A2C2-C39CD86D342E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5444" uniqueCount="1304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5444" uniqueCount="1305">
   <si>
     <t>Perennial horticulture</t>
   </si>
@@ -4175,12 +4175,15 @@
   <si>
     <t>T7.1 Annual croplands</t>
   </si>
+  <si>
+    <t>F3.2 Constructed lacustrine wetlands</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="55" x14ac:knownFonts="1">
+  <fonts count="56" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -4531,6 +4534,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="20">
     <fill>
@@ -4864,7 +4873,7 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5209,6 +5218,9 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -23326,8 +23338,8 @@
   <dimension ref="A1:N189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24:E185"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A171" sqref="A171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -29882,9 +29894,9 @@
         <v>6.2.1 Reservoir - mapping to IUCN GET - 169</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A171" t="str">
-        <f t="shared" si="4"/>
+        <f>CONCATENATE("alum:",LEFT(B171,FIND(" ",B171)-1))</f>
         <v>alum:6.2.2</v>
       </c>
       <c r="B171" t="s">
@@ -29896,8 +29908,8 @@
       <c r="D171" t="s">
         <v>1299</v>
       </c>
-      <c r="E171" t="s">
-        <v>1017</v>
+      <c r="E171" s="175" t="s">
+        <v>1304</v>
       </c>
       <c r="F171" s="154" t="s">
         <v>1033</v>
@@ -30672,15 +30684,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC29B5BE6945C34F8C7CB81794666E31" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f7151ef105987b2d3758ef53560e213">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48c5b5cd9b8d25ff6dd15848836f4270" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -30812,6 +30815,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -30822,14 +30834,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97EDE51C-194A-4D85-AD03-32004056A6AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30847,6 +30851,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Removed MFT1.3 Coastal saltmarshes and reedbeds from ALUM crosswalk.
</commit_message>
<xml_diff>
--- a/crosswalks/ALUM-IUCNGET/ALUM-IUCNGET.xlsx
+++ b/crosswalks/ALUM-IUCNGET/ALUM-IUCNGET.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60C02F5-ED80-4721-A2C2-C39CD86D342E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A7832F-00E1-4682-A845-398CCB5FFBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALUM V8" sheetId="5" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5444" uniqueCount="1305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5443" uniqueCount="1304">
   <si>
     <t>Perennial horticulture</t>
   </si>
@@ -4165,9 +4165,6 @@
   </si>
   <si>
     <t>get:groups/F3.5</t>
-  </si>
-  <si>
-    <t>get:groups/MFT1.3</t>
   </si>
   <si>
     <t>5.0.0 Intensive uses</t>
@@ -5189,6 +5186,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5218,9 +5218,6 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -5654,25 +5651,25 @@
     </row>
     <row r="2" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="165" t="s">
+      <c r="B2" s="166" t="s">
         <v>993</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
-      <c r="I2" s="165"/>
-      <c r="J2" s="165"/>
-      <c r="K2" s="165"/>
-      <c r="L2" s="165"/>
-      <c r="M2" s="165"/>
-      <c r="N2" s="165"/>
-      <c r="O2" s="165"/>
-      <c r="P2" s="165"/>
-      <c r="Q2" s="165"/>
-      <c r="R2" s="165"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
+      <c r="G2" s="166"/>
+      <c r="H2" s="166"/>
+      <c r="I2" s="166"/>
+      <c r="J2" s="166"/>
+      <c r="K2" s="166"/>
+      <c r="L2" s="166"/>
+      <c r="M2" s="166"/>
+      <c r="N2" s="166"/>
+      <c r="O2" s="166"/>
+      <c r="P2" s="166"/>
+      <c r="Q2" s="166"/>
+      <c r="R2" s="166"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8442,10 +8439,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CA0BFD-6560-4468-8D95-F8BDB1DE431A}">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8475,32 +8472,27 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>1023</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1303</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>1015</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A8" s="17" t="s">
         <v>1016</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A9">
-    <sortCondition ref="A1:A9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A8">
+    <sortCondition ref="A1:A8"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10968,25 +10960,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="167" t="s">
         <v>1005</v>
       </c>
-      <c r="B1" s="166"/>
-      <c r="C1" s="166"/>
-      <c r="D1" s="166"/>
-      <c r="E1" s="166"/>
-      <c r="F1" s="166"/>
-      <c r="G1" s="166"/>
-      <c r="H1" s="166"/>
-      <c r="I1" s="166"/>
-      <c r="J1" s="166"/>
-      <c r="K1" s="166"/>
-      <c r="O1" s="167" t="s">
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="167"/>
+      <c r="I1" s="167"/>
+      <c r="J1" s="167"/>
+      <c r="K1" s="167"/>
+      <c r="O1" s="168" t="s">
         <v>1005</v>
       </c>
-      <c r="P1" s="167"/>
-      <c r="Q1" s="167"/>
-      <c r="R1" s="167"/>
+      <c r="P1" s="168"/>
+      <c r="Q1" s="168"/>
+      <c r="R1" s="168"/>
       <c r="Y1" s="55"/>
       <c r="Z1" s="55"/>
       <c r="AA1" s="55"/>
@@ -11005,10 +10997,10 @@
       <c r="P2" s="126" t="s">
         <v>1007</v>
       </c>
-      <c r="Q2" s="167" t="s">
+      <c r="Q2" s="168" t="s">
         <v>951</v>
       </c>
-      <c r="R2" s="167"/>
+      <c r="R2" s="168"/>
       <c r="Y2" s="131" t="s">
         <v>960</v>
       </c>
@@ -11029,10 +11021,10 @@
       <c r="AO2" s="143" t="s">
         <v>960</v>
       </c>
-      <c r="AP2" s="169" t="s">
+      <c r="AP2" s="170" t="s">
         <v>1007</v>
       </c>
-      <c r="AQ2" s="169"/>
+      <c r="AQ2" s="170"/>
       <c r="AR2" s="144"/>
       <c r="AS2" s="144"/>
       <c r="AT2" s="145" t="s">
@@ -11099,10 +11091,10 @@
       <c r="AS3" s="141" t="s">
         <v>1009</v>
       </c>
-      <c r="AT3" s="168" t="s">
+      <c r="AT3" s="169" t="s">
         <v>946</v>
       </c>
-      <c r="AU3" s="168"/>
+      <c r="AU3" s="169"/>
       <c r="AV3" s="141" t="s">
         <v>947</v>
       </c>
@@ -14292,13 +14284,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="170"/>
-      <c r="B1" s="171"/>
-      <c r="C1" s="172" t="s">
+      <c r="A1" s="171"/>
+      <c r="B1" s="172"/>
+      <c r="C1" s="173" t="s">
         <v>659</v>
       </c>
-      <c r="D1" s="173"/>
-      <c r="E1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="175"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
@@ -19356,13 +19348,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="170"/>
-      <c r="B1" s="171"/>
-      <c r="C1" s="172" t="s">
+      <c r="A1" s="171"/>
+      <c r="B1" s="172"/>
+      <c r="C1" s="173" t="s">
         <v>659</v>
       </c>
-      <c r="D1" s="173"/>
-      <c r="E1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="175"/>
     </row>
     <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="109" t="s">
@@ -23337,9 +23329,9 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:N189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A171" sqref="A171"/>
+      <selection pane="bottomLeft" activeCell="E166" sqref="E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -24720,7 +24712,7 @@
         <v>1295</v>
       </c>
       <c r="E35" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F35" s="154" t="s">
         <v>1033</v>
@@ -24757,7 +24749,7 @@
         <v>1295</v>
       </c>
       <c r="E36" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F36" s="154" t="s">
         <v>1033</v>
@@ -24795,7 +24787,7 @@
         <v>1295</v>
       </c>
       <c r="E37" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F37" s="154" t="s">
         <v>1033</v>
@@ -24833,7 +24825,7 @@
         <v>1295</v>
       </c>
       <c r="E38" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F38" s="154" t="s">
         <v>1033</v>
@@ -24871,7 +24863,7 @@
         <v>1295</v>
       </c>
       <c r="E39" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F39" s="154" t="s">
         <v>1033</v>
@@ -24909,7 +24901,7 @@
         <v>1295</v>
       </c>
       <c r="E40" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F40" s="154" t="s">
         <v>1033</v>
@@ -24947,7 +24939,7 @@
         <v>1295</v>
       </c>
       <c r="E41" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F41" s="154" t="s">
         <v>1033</v>
@@ -24985,7 +24977,7 @@
         <v>1295</v>
       </c>
       <c r="E42" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F42" s="154" t="s">
         <v>1033</v>
@@ -25023,7 +25015,7 @@
         <v>1295</v>
       </c>
       <c r="E43" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F43" s="154" t="s">
         <v>1033</v>
@@ -25061,7 +25053,7 @@
         <v>1295</v>
       </c>
       <c r="E44" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F44" s="154" t="s">
         <v>1033</v>
@@ -25098,7 +25090,7 @@
         <v>1295</v>
       </c>
       <c r="E45" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F45" s="154" t="s">
         <v>1033</v>
@@ -25136,7 +25128,7 @@
         <v>1295</v>
       </c>
       <c r="E46" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F46" s="154" t="s">
         <v>1033</v>
@@ -25174,7 +25166,7 @@
         <v>1295</v>
       </c>
       <c r="E47" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F47" s="154" t="s">
         <v>1033</v>
@@ -25212,7 +25204,7 @@
         <v>1295</v>
       </c>
       <c r="E48" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F48" s="154" t="s">
         <v>1033</v>
@@ -25250,7 +25242,7 @@
         <v>1295</v>
       </c>
       <c r="E49" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F49" s="154" t="s">
         <v>1033</v>
@@ -25288,7 +25280,7 @@
         <v>1295</v>
       </c>
       <c r="E50" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F50" s="154" t="s">
         <v>1033</v>
@@ -25326,7 +25318,7 @@
         <v>1295</v>
       </c>
       <c r="E51" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F51" s="154" t="s">
         <v>1033</v>
@@ -25364,7 +25356,7 @@
         <v>1295</v>
       </c>
       <c r="E52" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F52" s="154" t="s">
         <v>1033</v>
@@ -25402,7 +25394,7 @@
         <v>1295</v>
       </c>
       <c r="E53" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F53" s="154" t="s">
         <v>1033</v>
@@ -25440,7 +25432,7 @@
         <v>1295</v>
       </c>
       <c r="E54" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F54" s="154" t="s">
         <v>1033</v>
@@ -25478,7 +25470,7 @@
         <v>1295</v>
       </c>
       <c r="E55" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F55" s="154" t="s">
         <v>1033</v>
@@ -25516,7 +25508,7 @@
         <v>1295</v>
       </c>
       <c r="E56" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F56" s="154" t="s">
         <v>1033</v>
@@ -26137,7 +26129,7 @@
         <v>1295</v>
       </c>
       <c r="E72" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F72" s="154" t="s">
         <v>1033</v>
@@ -26174,7 +26166,7 @@
         <v>1295</v>
       </c>
       <c r="E73" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F73" s="154" t="s">
         <v>1033</v>
@@ -26212,7 +26204,7 @@
         <v>1295</v>
       </c>
       <c r="E74" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F74" s="154" t="s">
         <v>1033</v>
@@ -26250,7 +26242,7 @@
         <v>1295</v>
       </c>
       <c r="E75" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F75" s="154" t="s">
         <v>1033</v>
@@ -26288,7 +26280,7 @@
         <v>1295</v>
       </c>
       <c r="E76" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F76" s="154" t="s">
         <v>1033</v>
@@ -26326,7 +26318,7 @@
         <v>1295</v>
       </c>
       <c r="E77" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F77" s="154" t="s">
         <v>1033</v>
@@ -26364,7 +26356,7 @@
         <v>1295</v>
       </c>
       <c r="E78" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F78" s="154" t="s">
         <v>1033</v>
@@ -26402,7 +26394,7 @@
         <v>1295</v>
       </c>
       <c r="E79" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F79" s="154" t="s">
         <v>1033</v>
@@ -26440,7 +26432,7 @@
         <v>1295</v>
       </c>
       <c r="E80" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F80" s="154" t="s">
         <v>1033</v>
@@ -26516,7 +26508,7 @@
         <v>1295</v>
       </c>
       <c r="E82" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F82" s="154" t="s">
         <v>1033</v>
@@ -26553,7 +26545,7 @@
         <v>1295</v>
       </c>
       <c r="E83" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F83" s="154" t="s">
         <v>1033</v>
@@ -26591,7 +26583,7 @@
         <v>1295</v>
       </c>
       <c r="E84" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F84" s="154" t="s">
         <v>1033</v>
@@ -26629,7 +26621,7 @@
         <v>1295</v>
       </c>
       <c r="E85" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F85" s="154" t="s">
         <v>1033</v>
@@ -26667,7 +26659,7 @@
         <v>1295</v>
       </c>
       <c r="E86" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F86" s="154" t="s">
         <v>1033</v>
@@ -26705,7 +26697,7 @@
         <v>1295</v>
       </c>
       <c r="E87" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F87" s="154" t="s">
         <v>1033</v>
@@ -26743,7 +26735,7 @@
         <v>1295</v>
       </c>
       <c r="E88" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F88" s="154" t="s">
         <v>1033</v>
@@ -26781,7 +26773,7 @@
         <v>1295</v>
       </c>
       <c r="E89" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F89" s="154" t="s">
         <v>1033</v>
@@ -26819,7 +26811,7 @@
         <v>1295</v>
       </c>
       <c r="E90" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F90" s="154" t="s">
         <v>1033</v>
@@ -26857,7 +26849,7 @@
         <v>1295</v>
       </c>
       <c r="E91" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F91" s="154" t="s">
         <v>1033</v>
@@ -26895,7 +26887,7 @@
         <v>1295</v>
       </c>
       <c r="E92" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F92" s="154" t="s">
         <v>1033</v>
@@ -26933,7 +26925,7 @@
         <v>1295</v>
       </c>
       <c r="E93" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F93" s="154" t="s">
         <v>1033</v>
@@ -26971,7 +26963,7 @@
         <v>1295</v>
       </c>
       <c r="E94" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F94" s="154" t="s">
         <v>1033</v>
@@ -27009,7 +27001,7 @@
         <v>1295</v>
       </c>
       <c r="E95" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="F95" s="154" t="s">
         <v>1033</v>
@@ -27243,7 +27235,7 @@
         <v>alum:5.0.0</v>
       </c>
       <c r="B101" s="17" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="C101" s="164" t="s">
         <v>1030</v>
@@ -29908,8 +29900,8 @@
       <c r="D171" t="s">
         <v>1299</v>
       </c>
-      <c r="E171" s="175" t="s">
-        <v>1304</v>
+      <c r="E171" s="165" t="s">
+        <v>1303</v>
       </c>
       <c r="F171" s="154" t="s">
         <v>1033</v>
@@ -30449,14 +30441,14 @@
       <c r="B185" t="s">
         <v>1222</v>
       </c>
-      <c r="C185" t="s">
-        <v>1031</v>
-      </c>
-      <c r="D185" t="s">
-        <v>1301</v>
-      </c>
-      <c r="E185" t="s">
-        <v>1023</v>
+      <c r="C185" s="104" t="s">
+        <v>1030</v>
+      </c>
+      <c r="D185" s="104" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E185" s="104" t="s">
+        <v>1046</v>
       </c>
       <c r="F185" s="154" t="s">
         <v>1033</v>
@@ -30684,6 +30676,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC29B5BE6945C34F8C7CB81794666E31" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f7151ef105987b2d3758ef53560e213">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48c5b5cd9b8d25ff6dd15848836f4270" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -30815,25 +30825,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97EDE51C-194A-4D85-AD03-32004056A6AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30849,22 +30859,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated ALUM Xwalk from Anna.
</commit_message>
<xml_diff>
--- a/crosswalks/ALUM-IUCNGET/ALUM-IUCNGET.xlsx
+++ b/crosswalks/ALUM-IUCNGET/ALUM-IUCNGET.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A7832F-00E1-4682-A845-398CCB5FFBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FA19D5F-AE37-4CF7-A308-A4B071456F77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ALUM V8" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,20 @@
     <definedName name="Z_AB65B437_1B49_4040_B070_7D10DCCE9FB5_.wvu.PrintArea" localSheetId="0" hidden="1">'ALUM V8'!$A$1:$S$75</definedName>
     <definedName name="Z_E13C975D_9911_46DF_BB53_0E45A3160659_.wvu.PrintArea" localSheetId="0" hidden="1">'ALUM V8'!$A$1:$S$77</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -63,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5443" uniqueCount="1304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5446" uniqueCount="1306">
   <si>
     <t>Perennial horticulture</t>
   </si>
@@ -4174,6 +4187,12 @@
   </si>
   <si>
     <t>F3.2 Constructed lacustrine wetlands</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Updated the cross-walk from the teams site version with Suzanne and David's comments</t>
   </si>
 </sst>
 </file>
@@ -4870,7 +4889,7 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -5186,9 +5205,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5219,6 +5235,12 @@
     <xf numFmtId="0" fontId="31" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
@@ -5230,7 +5252,21 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="7" xr:uid="{6E4AE3D0-7BAA-41EF-A73F-6403105D203D}"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5651,25 +5687,25 @@
     </row>
     <row r="2" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="166" t="s">
+      <c r="B2" s="165" t="s">
         <v>993</v>
       </c>
-      <c r="C2" s="166"/>
-      <c r="D2" s="166"/>
-      <c r="E2" s="166"/>
-      <c r="F2" s="166"/>
-      <c r="G2" s="166"/>
-      <c r="H2" s="166"/>
-      <c r="I2" s="166"/>
-      <c r="J2" s="166"/>
-      <c r="K2" s="166"/>
-      <c r="L2" s="166"/>
-      <c r="M2" s="166"/>
-      <c r="N2" s="166"/>
-      <c r="O2" s="166"/>
-      <c r="P2" s="166"/>
-      <c r="Q2" s="166"/>
-      <c r="R2" s="166"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="165"/>
+      <c r="H2" s="165"/>
+      <c r="I2" s="165"/>
+      <c r="J2" s="165"/>
+      <c r="K2" s="165"/>
+      <c r="L2" s="165"/>
+      <c r="M2" s="165"/>
+      <c r="N2" s="165"/>
+      <c r="O2" s="165"/>
+      <c r="P2" s="165"/>
+      <c r="Q2" s="165"/>
+      <c r="R2" s="165"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8335,10 +8371,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655D2789-1FB8-4FE0-B6BE-798F6232EAF5}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8432,6 +8468,20 @@
         <v>1066</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="152">
+        <v>45513</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1304</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>1066</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8441,7 +8491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CA0BFD-6560-4468-8D95-F8BDB1DE431A}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -10960,25 +11010,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.2">
-      <c r="A1" s="167" t="s">
+      <c r="A1" s="166" t="s">
         <v>1005</v>
       </c>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="167"/>
-      <c r="J1" s="167"/>
-      <c r="K1" s="167"/>
-      <c r="O1" s="168" t="s">
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="166"/>
+      <c r="O1" s="167" t="s">
         <v>1005</v>
       </c>
-      <c r="P1" s="168"/>
-      <c r="Q1" s="168"/>
-      <c r="R1" s="168"/>
+      <c r="P1" s="167"/>
+      <c r="Q1" s="167"/>
+      <c r="R1" s="167"/>
       <c r="Y1" s="55"/>
       <c r="Z1" s="55"/>
       <c r="AA1" s="55"/>
@@ -10997,10 +11047,10 @@
       <c r="P2" s="126" t="s">
         <v>1007</v>
       </c>
-      <c r="Q2" s="168" t="s">
+      <c r="Q2" s="167" t="s">
         <v>951</v>
       </c>
-      <c r="R2" s="168"/>
+      <c r="R2" s="167"/>
       <c r="Y2" s="131" t="s">
         <v>960</v>
       </c>
@@ -11021,10 +11071,10 @@
       <c r="AO2" s="143" t="s">
         <v>960</v>
       </c>
-      <c r="AP2" s="170" t="s">
+      <c r="AP2" s="169" t="s">
         <v>1007</v>
       </c>
-      <c r="AQ2" s="170"/>
+      <c r="AQ2" s="169"/>
       <c r="AR2" s="144"/>
       <c r="AS2" s="144"/>
       <c r="AT2" s="145" t="s">
@@ -11091,10 +11141,10 @@
       <c r="AS3" s="141" t="s">
         <v>1009</v>
       </c>
-      <c r="AT3" s="169" t="s">
+      <c r="AT3" s="168" t="s">
         <v>946</v>
       </c>
-      <c r="AU3" s="169"/>
+      <c r="AU3" s="168"/>
       <c r="AV3" s="141" t="s">
         <v>947</v>
       </c>
@@ -14284,13 +14334,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="171"/>
-      <c r="B1" s="172"/>
-      <c r="C1" s="173" t="s">
+      <c r="A1" s="170"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="172" t="s">
         <v>659</v>
       </c>
-      <c r="D1" s="174"/>
-      <c r="E1" s="175"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="174"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
@@ -19348,13 +19398,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="171"/>
-      <c r="B1" s="172"/>
-      <c r="C1" s="173" t="s">
+      <c r="A1" s="170"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="172" t="s">
         <v>659</v>
       </c>
-      <c r="D1" s="174"/>
-      <c r="E1" s="175"/>
+      <c r="D1" s="173"/>
+      <c r="E1" s="174"/>
     </row>
     <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="109" t="s">
@@ -23329,9 +23379,9 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:N189"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E166" sqref="E166"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -24133,13 +24183,13 @@
       <c r="B20" t="s">
         <v>1228</v>
       </c>
-      <c r="C20" s="157" t="s">
+      <c r="C20" s="176" t="s">
         <v>1030</v>
       </c>
-      <c r="D20" s="157" t="s">
+      <c r="D20" s="176" t="s">
         <v>1045</v>
       </c>
-      <c r="E20" s="157" t="s">
+      <c r="E20" s="176" t="s">
         <v>1046</v>
       </c>
       <c r="F20" s="154" t="s">
@@ -25053,7 +25103,7 @@
         <v>1295</v>
       </c>
       <c r="E44" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F44" s="154" t="s">
         <v>1033</v>
@@ -25090,7 +25140,7 @@
         <v>1295</v>
       </c>
       <c r="E45" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F45" s="154" t="s">
         <v>1033</v>
@@ -25128,7 +25178,7 @@
         <v>1295</v>
       </c>
       <c r="E46" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F46" s="154" t="s">
         <v>1033</v>
@@ -25166,7 +25216,7 @@
         <v>1295</v>
       </c>
       <c r="E47" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F47" s="154" t="s">
         <v>1033</v>
@@ -25204,7 +25254,7 @@
         <v>1295</v>
       </c>
       <c r="E48" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F48" s="154" t="s">
         <v>1033</v>
@@ -25242,7 +25292,7 @@
         <v>1295</v>
       </c>
       <c r="E49" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F49" s="154" t="s">
         <v>1033</v>
@@ -25356,7 +25406,7 @@
         <v>1295</v>
       </c>
       <c r="E52" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F52" s="154" t="s">
         <v>1033</v>
@@ -25394,7 +25444,7 @@
         <v>1295</v>
       </c>
       <c r="E53" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F53" s="154" t="s">
         <v>1033</v>
@@ -26508,7 +26558,7 @@
         <v>1295</v>
       </c>
       <c r="E82" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F82" s="154" t="s">
         <v>1033</v>
@@ -26545,7 +26595,7 @@
         <v>1295</v>
       </c>
       <c r="E83" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F83" s="154" t="s">
         <v>1033</v>
@@ -26583,7 +26633,7 @@
         <v>1295</v>
       </c>
       <c r="E84" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F84" s="154" t="s">
         <v>1033</v>
@@ -26621,7 +26671,7 @@
         <v>1295</v>
       </c>
       <c r="E85" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F85" s="154" t="s">
         <v>1033</v>
@@ -26659,7 +26709,7 @@
         <v>1295</v>
       </c>
       <c r="E86" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F86" s="154" t="s">
         <v>1033</v>
@@ -26697,7 +26747,7 @@
         <v>1295</v>
       </c>
       <c r="E87" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F87" s="154" t="s">
         <v>1033</v>
@@ -26811,7 +26861,7 @@
         <v>1295</v>
       </c>
       <c r="E90" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F90" s="154" t="s">
         <v>1033</v>
@@ -26849,7 +26899,7 @@
         <v>1295</v>
       </c>
       <c r="E91" t="s">
-        <v>1302</v>
+        <v>1015</v>
       </c>
       <c r="F91" s="154" t="s">
         <v>1033</v>
@@ -29886,7 +29936,7 @@
         <v>6.2.1 Reservoir - mapping to IUCN GET - 169</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A171" t="str">
         <f>CONCATENATE("alum:",LEFT(B171,FIND(" ",B171)-1))</f>
         <v>alum:6.2.2</v>
@@ -29900,7 +29950,7 @@
       <c r="D171" t="s">
         <v>1299</v>
       </c>
-      <c r="E171" s="165" t="s">
+      <c r="E171" s="175" t="s">
         <v>1303</v>
       </c>
       <c r="F171" s="154" t="s">
@@ -29939,7 +29989,7 @@
         <v>1299</v>
       </c>
       <c r="E172" t="s">
-        <v>1017</v>
+        <v>1303</v>
       </c>
       <c r="F172" s="154" t="s">
         <v>1033</v>
@@ -30636,38 +30686,48 @@
     <sortCondition ref="B2:B189"/>
   </sortState>
   <conditionalFormatting sqref="C2:E20">
-    <cfRule type="containsBlanks" dxfId="6" priority="1">
+    <cfRule type="containsBlanks" dxfId="8" priority="3">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:E53">
-    <cfRule type="containsBlanks" dxfId="5" priority="11">
+  <conditionalFormatting sqref="C49:D53">
+    <cfRule type="containsBlanks" dxfId="7" priority="13">
       <formula>LEN(TRIM(C49))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C84:E88">
-    <cfRule type="containsBlanks" dxfId="4" priority="10">
+  <conditionalFormatting sqref="C84:D88">
+    <cfRule type="containsBlanks" dxfId="6" priority="12">
       <formula>LEN(TRIM(C84))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C159:E161">
-    <cfRule type="containsBlanks" dxfId="3" priority="9">
+    <cfRule type="containsBlanks" dxfId="5" priority="11">
       <formula>LEN(TRIM(C159))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D142:E145">
-    <cfRule type="containsBlanks" dxfId="2" priority="4">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(D142))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D149:E151">
-    <cfRule type="containsBlanks" dxfId="1" priority="7">
+    <cfRule type="containsBlanks" dxfId="3" priority="9">
       <formula>LEN(TRIM(D149))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D155:E156">
-    <cfRule type="containsBlanks" dxfId="0" priority="6">
+    <cfRule type="containsBlanks" dxfId="2" priority="8">
       <formula>LEN(TRIM(D155))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49 E52:E53">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(E49))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E84:E87">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(E84))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30676,24 +30736,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DC29B5BE6945C34F8C7CB81794666E31" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9f7151ef105987b2d3758ef53560e213">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="48c5b5cd9b8d25ff6dd15848836f4270" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -30825,25 +30867,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97EDE51C-194A-4D85-AD03-32004056A6AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -30859,4 +30901,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8BEB67B5-0F24-4813-B2D2-A92E60BF00F8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64B25D3-7183-4323-848D-DB8D888013A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>